<commit_message>
add mock for AuditorReplicasCheckTest.java
</commit_message>
<xml_diff>
--- a/test-poly-inheritance.xlsx
+++ b/test-poly-inheritance.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-rule-space\projects\bookkeeper_mocking_refactoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B31BCC5-D4D8-41B5-B278-DE784C27A434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0279B2CB-4FBA-4AF6-B9CC-8E17699C1265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3264" windowWidth="7500" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3264" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test-poly-inheritance" sheetId="1" r:id="rId1"/>
@@ -1227,7 +1227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2061,7 +2061,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I377"/>
   <sheetViews>
@@ -13014,7 +13014,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I377">
+  <autoFilter ref="A1:I377" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="inheritProduction"/>
@@ -13026,11 +13026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16409,11 +16409,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1">
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I116">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>